<commit_message>
Misc updates to outputs
</commit_message>
<xml_diff>
--- a/Data/Reach_Assessments_Projects_Table_05052020.xlsx
+++ b/Data/Reach_Assessments_Projects_Table_05052020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E9C586-55A0-4F53-848C-E7002739B734}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE0B71B-CA7B-434C-B18A-6F8CC225BC4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="19680" windowHeight="11016" xr2:uid="{431DE12E-E4F2-45D1-A6E0-EFCBE1121B10}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="21972" windowHeight="11796" xr2:uid="{431DE12E-E4F2-45D1-A6E0-EFCBE1121B10}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Entry" sheetId="1" r:id="rId1"/>
@@ -7264,7 +7264,7 @@
     <t>Side Channel and Off-Channel Habitat Restoration</t>
   </si>
   <si>
-    <t>Middle Methow Reach Assessment</t>
+    <t>Methow River Project Opportunity Assessment - Twisp River to Lewisia Road</t>
   </si>
 </sst>
 </file>
@@ -8799,9 +8799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27050BFB-5885-470D-AF38-F49DD2A4C41F}">
   <dimension ref="A1:X2235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A988" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C996" sqref="C996"/>
+      <selection pane="bottomLeft" activeCell="B994" sqref="B994"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20399,7 +20399,7 @@
       </c>
       <c r="K366" s="11"/>
       <c r="O366" s="2">
-        <f>3.55-2.15</f>
+        <f t="shared" ref="O366:O371" si="0">3.55-2.15</f>
         <v>1.4</v>
       </c>
     </row>
@@ -20430,7 +20430,7 @@
       </c>
       <c r="K367" s="11"/>
       <c r="O367" s="2">
-        <f>3.55-2.15</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
     </row>
@@ -20461,7 +20461,7 @@
       </c>
       <c r="K368" s="11"/>
       <c r="O368" s="2">
-        <f>3.55-2.15</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
     </row>
@@ -20492,7 +20492,7 @@
       </c>
       <c r="K369" s="11"/>
       <c r="O369" s="2">
-        <f>3.55-2.15</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
     </row>
@@ -20523,7 +20523,7 @@
       </c>
       <c r="K370" s="11"/>
       <c r="O370" s="2">
-        <f>3.55-2.15</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
     </row>
@@ -20554,7 +20554,7 @@
       </c>
       <c r="K371" s="11"/>
       <c r="O371" s="2">
-        <f>3.55-2.15</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
     </row>
@@ -74438,7 +74438,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74452,7 +74452,7 @@
     <col min="7" max="7" width="33" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="34.88671875" customWidth="1"/>
     <col min="11" max="11" width="44" customWidth="1"/>
     <col min="12" max="12" width="24.6640625" customWidth="1"/>
     <col min="13" max="13" width="28.88671875" customWidth="1"/>

</xml_diff>